<commit_message>
chapter 4 output sets
</commit_message>
<xml_diff>
--- a/datasets/Ch4/boxoffice_by_month.xlsx
+++ b/datasets/Ch4/boxoffice_by_month.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="April" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="August" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="July" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="June" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="May" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="April" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="August" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="July" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="June" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="May" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,9 +20,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="MM-DD-YYYY"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -67,7 +68,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>